<commit_message>
Docu update on daily_log and deliverables
</commit_message>
<xml_diff>
--- a/Documentation/Daily_Log.xlsx
+++ b/Documentation/Daily_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\NutriWISE\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1F5A4-70FF-40F0-8F52-85813B81073D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F47FCDE-5E6C-4BFD-995E-EE66F0298174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7995C46D-4874-4851-BB31-44BEABCE427D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7995C46D-4874-4851-BB31-44BEABCE427D}"/>
   </bookViews>
   <sheets>
     <sheet name="June 20-2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Daily Log</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Jephthah  Jehosaphat Landicho</t>
+  </si>
+  <si>
+    <t>Added functionality on "meal plan" button.</t>
+  </si>
+  <si>
+    <t>"Meal plan " button consisting of client name, assessor, and the entire meal plan</t>
+  </si>
+  <si>
+    <t>The "view meal plan" button gives a detailed meal plan.</t>
   </si>
 </sst>
 </file>
@@ -493,13 +502,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C963E2-42FE-48A7-854D-517B66E8FC07}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
@@ -602,13 +612,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44901C3-5F03-4C62-9FB1-465A48DD5BD0}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
@@ -647,15 +658,24 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Docu update on daily log
</commit_message>
<xml_diff>
--- a/Documentation/Daily_Log.xlsx
+++ b/Documentation/Daily_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\NutriWISE\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F47FCDE-5E6C-4BFD-995E-EE66F0298174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10288E4-0C36-46AD-9C3B-5C4A8ACEF895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7995C46D-4874-4851-BB31-44BEABCE427D}"/>
   </bookViews>
@@ -17,6 +17,10 @@
     <sheet name="June 21-2023" sheetId="5" r:id="rId2"/>
     <sheet name="June 22-2023" sheetId="9" r:id="rId3"/>
     <sheet name="June 23-2023" sheetId="10" r:id="rId4"/>
+    <sheet name="June 24-2023" sheetId="12" r:id="rId5"/>
+    <sheet name="June 25-2023" sheetId="13" r:id="rId6"/>
+    <sheet name="June 26-2023" sheetId="14" r:id="rId7"/>
+    <sheet name="June 27-2023" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
   <si>
     <t>Daily Log</t>
   </si>
@@ -94,6 +98,9 @@
   </si>
   <si>
     <t>The "view meal plan" button gives a detailed meal plan.</t>
+  </si>
+  <si>
+    <t>added functionality of food exchange computation.</t>
   </si>
 </sst>
 </file>
@@ -613,7 +620,7 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,6 +689,9 @@
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -859,4 +869,328 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FADBB79-5D9A-48BA-A917-B31D85393509}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB875078-A22D-48DA-90E0-02E84015FA53}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D434C-F42B-4874-B5BA-141DFE28FC39}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA46051F-245F-4785-9FB5-BE6DCE96C517}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="24.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>